<commit_message>
nabkisan Early repay sce
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Loan Product/Scenario1-NABKISAN-EARLY-TR1-Loanproduct.xlsx
+++ b/Mifos Automation Excels/Loan Product/Scenario1-NABKISAN-EARLY-TR1-Loanproduct.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>productname</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Scenario1-NABKISAN-EARLY-TR1</t>
+  </si>
+  <si>
+    <t>t1</t>
   </si>
 </sst>
 </file>
@@ -536,7 +539,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -557,8 +560,8 @@
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
-        <v>1</v>
+      <c r="B2" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -606,7 +609,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2">
-        <v>30000000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -622,7 +625,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -790,7 +793,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="7">
-        <v>30000000</v>
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>
@@ -804,7 +807,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>